<commit_message>
jwt ile rolleme işlemi tamamlandı, mantıksal düzeltmeler yapılacak
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -260,12 +260,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -605,7 +606,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D284"/>
+  <dimension ref="A1:D319"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -4595,6 +4596,496 @@
         <v>45597.0</v>
       </c>
     </row>
+    <row r="285">
+      <c r="A285" t="n" s="0">
+        <v>442.0</v>
+      </c>
+      <c r="B285" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C285" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D285" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n" s="0">
+        <v>443.0</v>
+      </c>
+      <c r="B286" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C286" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D286" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n" s="0">
+        <v>444.0</v>
+      </c>
+      <c r="B287" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C287" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D287" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n" s="0">
+        <v>445.0</v>
+      </c>
+      <c r="B288" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C288" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D288" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n" s="0">
+        <v>446.0</v>
+      </c>
+      <c r="B289" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C289" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D289" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n" s="0">
+        <v>447.0</v>
+      </c>
+      <c r="B290" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C290" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D290" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n" s="0">
+        <v>448.0</v>
+      </c>
+      <c r="B291" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C291" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D291" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n" s="0">
+        <v>449.0</v>
+      </c>
+      <c r="B292" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C292" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D292" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n" s="0">
+        <v>450.0</v>
+      </c>
+      <c r="B293" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C293" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D293" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n" s="0">
+        <v>451.0</v>
+      </c>
+      <c r="B294" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C294" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D294" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n" s="0">
+        <v>452.0</v>
+      </c>
+      <c r="B295" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C295" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D295" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n" s="0">
+        <v>453.0</v>
+      </c>
+      <c r="B296" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C296" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D296" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n" s="0">
+        <v>454.0</v>
+      </c>
+      <c r="B297" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C297" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D297" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n" s="0">
+        <v>455.0</v>
+      </c>
+      <c r="B298" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C298" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D298" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n" s="0">
+        <v>456.0</v>
+      </c>
+      <c r="B299" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C299" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D299" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n" s="0">
+        <v>457.0</v>
+      </c>
+      <c r="B300" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C300" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D300" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n" s="0">
+        <v>458.0</v>
+      </c>
+      <c r="B301" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C301" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D301" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n" s="0">
+        <v>459.0</v>
+      </c>
+      <c r="B302" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C302" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D302" t="n" s="8">
+        <v>45597.0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n" s="0">
+        <v>460.0</v>
+      </c>
+      <c r="B303" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C303" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D303" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n" s="0">
+        <v>461.0</v>
+      </c>
+      <c r="B304" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C304" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D304" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n" s="0">
+        <v>462.0</v>
+      </c>
+      <c r="B305" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C305" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D305" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n" s="0">
+        <v>463.0</v>
+      </c>
+      <c r="B306" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C306" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D306" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n" s="0">
+        <v>464.0</v>
+      </c>
+      <c r="B307" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C307" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D307" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n" s="0">
+        <v>465.0</v>
+      </c>
+      <c r="B308" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C308" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D308" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n" s="0">
+        <v>466.0</v>
+      </c>
+      <c r="B309" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C309" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D309" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n" s="0">
+        <v>467.0</v>
+      </c>
+      <c r="B310" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C310" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D310" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n" s="0">
+        <v>468.0</v>
+      </c>
+      <c r="B311" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C311" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D311" t="n" s="8">
+        <v>45599.0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n" s="0">
+        <v>469.0</v>
+      </c>
+      <c r="B312" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C312" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D312" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n" s="0">
+        <v>470.0</v>
+      </c>
+      <c r="B313" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C313" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D313" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n" s="0">
+        <v>471.0</v>
+      </c>
+      <c r="B314" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C314" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D314" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n" s="0">
+        <v>472.0</v>
+      </c>
+      <c r="B315" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C315" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D315" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n" s="0">
+        <v>473.0</v>
+      </c>
+      <c r="B316" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C316" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="D316" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n" s="0">
+        <v>474.0</v>
+      </c>
+      <c r="B317" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C317" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="D317" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n" s="0">
+        <v>475.0</v>
+      </c>
+      <c r="B318" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C318" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D318" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n" s="0">
+        <v>476.0</v>
+      </c>
+      <c r="B319" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C319" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D319" t="n" s="8">
+        <v>45600.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ceza tanımları ayrı bir tabloda da tutulacağı için ceza tablosundaki bazı sütunlar silindi ve ceza tanımları tablosu, dto'su ve mapper'ı oluşturuldu
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -260,12 +260,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -606,7 +607,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D319"/>
+  <dimension ref="A1:D329"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -5086,6 +5087,146 @@
         <v>45600.0</v>
       </c>
     </row>
+    <row r="320">
+      <c r="A320" t="n" s="0">
+        <v>625.0</v>
+      </c>
+      <c r="B320" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C320" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D320" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n" s="0">
+        <v>626.0</v>
+      </c>
+      <c r="B321" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C321" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D321" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n" s="0">
+        <v>627.0</v>
+      </c>
+      <c r="B322" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C322" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D322" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n" s="0">
+        <v>628.0</v>
+      </c>
+      <c r="B323" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C323" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D323" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n" s="0">
+        <v>629.0</v>
+      </c>
+      <c r="B324" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C324" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D324" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n" s="0">
+        <v>630.0</v>
+      </c>
+      <c r="B325" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C325" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D325" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n" s="0">
+        <v>631.0</v>
+      </c>
+      <c r="B326" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C326" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D326" t="n" s="9">
+        <v>45611.0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n" s="0">
+        <v>632.0</v>
+      </c>
+      <c r="B327" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C327" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D327" t="n" s="9">
+        <v>45614.0</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n" s="0">
+        <v>633.0</v>
+      </c>
+      <c r="B328" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C328" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D328" t="n" s="9">
+        <v>45614.0</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n" s="0">
+        <v>634.0</v>
+      </c>
+      <c r="B329" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C329" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D329" t="n" s="9">
+        <v>45615.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Öğrenciyi odaya yerleştirme ve tüm koşulları(odadaki öğrenci sayısını arttırma, dolduysa isFull değerine true yapma ve doluysa ekleme hayası verme) yapıldı
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -260,12 +260,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -607,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D329"/>
+  <dimension ref="A1:D333"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -5227,6 +5228,62 @@
         <v>45615.0</v>
       </c>
     </row>
+    <row r="330">
+      <c r="A330" t="n" s="0">
+        <v>635.0</v>
+      </c>
+      <c r="B330" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C330" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D330" t="n" s="10">
+        <v>45616.0</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n" s="0">
+        <v>636.0</v>
+      </c>
+      <c r="B331" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C331" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D331" t="n" s="10">
+        <v>45616.0</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n" s="0">
+        <v>637.0</v>
+      </c>
+      <c r="B332" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C332" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D332" t="n" s="10">
+        <v>45616.0</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n" s="0">
+        <v>638.0</v>
+      </c>
+      <c r="B333" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C333" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D333" t="n" s="10">
+        <v>45616.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tabloların yarısı mongoDb ye aktarıldı
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Spor türü ekleme işlemi başarılı</t>
+  </si>
+  <si>
+    <t>Tüm öğrencilerin listelenmesinde bir hata oluştu</t>
   </si>
 </sst>
 </file>
@@ -260,12 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -608,7 +612,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D333"/>
+  <dimension ref="A1:D340"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -5284,6 +5288,104 @@
         <v>45616.0</v>
       </c>
     </row>
+    <row r="334">
+      <c r="A334" t="n" s="0">
+        <v>639.0</v>
+      </c>
+      <c r="B334" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C334" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="D334" t="n" s="11">
+        <v>45618.0</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n" s="0">
+        <v>640.0</v>
+      </c>
+      <c r="B335" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C335" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="D335" t="n" s="11">
+        <v>45618.0</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n" s="0">
+        <v>641.0</v>
+      </c>
+      <c r="B336" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C336" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="D336" t="n" s="11">
+        <v>45618.0</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n" s="0">
+        <v>642.0</v>
+      </c>
+      <c r="B337" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C337" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="D337" t="n" s="11">
+        <v>45618.0</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n" s="0">
+        <v>643.0</v>
+      </c>
+      <c r="B338" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C338" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D338" t="n" s="11">
+        <v>45618.0</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n" s="0">
+        <v>644.0</v>
+      </c>
+      <c r="B339" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C339" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D339" t="n" s="11">
+        <v>45618.0</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n" s="0">
+        <v>645.0</v>
+      </c>
+      <c r="B340" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C340" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D340" t="n" s="11">
+        <v>45621.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AuthController ve JWTGenerator kısmında rolü payload a yükledim
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -263,12 +263,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -612,7 +615,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D340"/>
+  <dimension ref="A1:D671"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -5386,6 +5389,4640 @@
         <v>45621.0</v>
       </c>
     </row>
+    <row r="341">
+      <c r="A341" t="n" s="0">
+        <v>646.0</v>
+      </c>
+      <c r="B341" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C341" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D341" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n" s="0">
+        <v>647.0</v>
+      </c>
+      <c r="B342" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C342" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D342" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n" s="0">
+        <v>648.0</v>
+      </c>
+      <c r="B343" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C343" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D343" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n" s="0">
+        <v>649.0</v>
+      </c>
+      <c r="B344" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C344" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D344" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n" s="0">
+        <v>650.0</v>
+      </c>
+      <c r="B345" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C345" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D345" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n" s="0">
+        <v>651.0</v>
+      </c>
+      <c r="B346" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C346" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D346" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n" s="0">
+        <v>652.0</v>
+      </c>
+      <c r="B347" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C347" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D347" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n" s="0">
+        <v>653.0</v>
+      </c>
+      <c r="B348" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C348" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D348" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n" s="0">
+        <v>654.0</v>
+      </c>
+      <c r="B349" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C349" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D349" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n" s="0">
+        <v>655.0</v>
+      </c>
+      <c r="B350" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C350" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D350" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n" s="0">
+        <v>656.0</v>
+      </c>
+      <c r="B351" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C351" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D351" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n" s="0">
+        <v>657.0</v>
+      </c>
+      <c r="B352" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C352" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D352" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n" s="0">
+        <v>658.0</v>
+      </c>
+      <c r="B353" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C353" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D353" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n" s="0">
+        <v>659.0</v>
+      </c>
+      <c r="B354" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C354" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D354" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n" s="0">
+        <v>660.0</v>
+      </c>
+      <c r="B355" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C355" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D355" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n" s="0">
+        <v>661.0</v>
+      </c>
+      <c r="B356" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C356" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D356" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n" s="0">
+        <v>662.0</v>
+      </c>
+      <c r="B357" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C357" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D357" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n" s="0">
+        <v>663.0</v>
+      </c>
+      <c r="B358" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C358" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D358" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n" s="0">
+        <v>664.0</v>
+      </c>
+      <c r="B359" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C359" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D359" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n" s="0">
+        <v>665.0</v>
+      </c>
+      <c r="B360" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C360" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D360" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n" s="0">
+        <v>666.0</v>
+      </c>
+      <c r="B361" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C361" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D361" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n" s="0">
+        <v>667.0</v>
+      </c>
+      <c r="B362" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C362" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D362" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n" s="0">
+        <v>668.0</v>
+      </c>
+      <c r="B363" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C363" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D363" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n" s="0">
+        <v>669.0</v>
+      </c>
+      <c r="B364" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C364" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D364" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n" s="0">
+        <v>670.0</v>
+      </c>
+      <c r="B365" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C365" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D365" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n" s="0">
+        <v>671.0</v>
+      </c>
+      <c r="B366" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C366" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D366" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n" s="0">
+        <v>672.0</v>
+      </c>
+      <c r="B367" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C367" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D367" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n" s="0">
+        <v>673.0</v>
+      </c>
+      <c r="B368" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C368" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D368" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n" s="0">
+        <v>674.0</v>
+      </c>
+      <c r="B369" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C369" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D369" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n" s="0">
+        <v>675.0</v>
+      </c>
+      <c r="B370" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C370" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D370" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n" s="0">
+        <v>676.0</v>
+      </c>
+      <c r="B371" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C371" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D371" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n" s="0">
+        <v>677.0</v>
+      </c>
+      <c r="B372" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C372" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D372" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n" s="0">
+        <v>678.0</v>
+      </c>
+      <c r="B373" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C373" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D373" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n" s="0">
+        <v>679.0</v>
+      </c>
+      <c r="B374" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C374" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D374" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n" s="0">
+        <v>680.0</v>
+      </c>
+      <c r="B375" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C375" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D375" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n" s="0">
+        <v>681.0</v>
+      </c>
+      <c r="B376" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C376" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D376" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n" s="0">
+        <v>682.0</v>
+      </c>
+      <c r="B377" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C377" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D377" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n" s="0">
+        <v>683.0</v>
+      </c>
+      <c r="B378" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C378" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D378" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n" s="0">
+        <v>684.0</v>
+      </c>
+      <c r="B379" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C379" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D379" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n" s="0">
+        <v>685.0</v>
+      </c>
+      <c r="B380" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C380" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D380" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n" s="0">
+        <v>686.0</v>
+      </c>
+      <c r="B381" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C381" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D381" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n" s="0">
+        <v>687.0</v>
+      </c>
+      <c r="B382" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C382" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D382" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n" s="0">
+        <v>688.0</v>
+      </c>
+      <c r="B383" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C383" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D383" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n" s="0">
+        <v>689.0</v>
+      </c>
+      <c r="B384" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C384" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D384" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n" s="0">
+        <v>690.0</v>
+      </c>
+      <c r="B385" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C385" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D385" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n" s="0">
+        <v>691.0</v>
+      </c>
+      <c r="B386" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C386" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D386" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n" s="0">
+        <v>692.0</v>
+      </c>
+      <c r="B387" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C387" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D387" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n" s="0">
+        <v>693.0</v>
+      </c>
+      <c r="B388" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C388" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D388" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n" s="0">
+        <v>694.0</v>
+      </c>
+      <c r="B389" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C389" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D389" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n" s="0">
+        <v>695.0</v>
+      </c>
+      <c r="B390" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C390" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D390" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n" s="0">
+        <v>696.0</v>
+      </c>
+      <c r="B391" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C391" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D391" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n" s="0">
+        <v>697.0</v>
+      </c>
+      <c r="B392" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C392" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D392" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n" s="0">
+        <v>698.0</v>
+      </c>
+      <c r="B393" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C393" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D393" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n" s="0">
+        <v>699.0</v>
+      </c>
+      <c r="B394" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C394" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D394" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n" s="0">
+        <v>700.0</v>
+      </c>
+      <c r="B395" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C395" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D395" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n" s="0">
+        <v>701.0</v>
+      </c>
+      <c r="B396" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C396" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D396" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n" s="0">
+        <v>702.0</v>
+      </c>
+      <c r="B397" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C397" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D397" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n" s="0">
+        <v>703.0</v>
+      </c>
+      <c r="B398" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C398" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D398" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n" s="0">
+        <v>704.0</v>
+      </c>
+      <c r="B399" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C399" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D399" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n" s="0">
+        <v>705.0</v>
+      </c>
+      <c r="B400" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C400" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D400" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n" s="0">
+        <v>706.0</v>
+      </c>
+      <c r="B401" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C401" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D401" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n" s="0">
+        <v>707.0</v>
+      </c>
+      <c r="B402" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C402" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D402" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n" s="0">
+        <v>708.0</v>
+      </c>
+      <c r="B403" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C403" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D403" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n" s="0">
+        <v>709.0</v>
+      </c>
+      <c r="B404" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C404" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D404" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n" s="0">
+        <v>710.0</v>
+      </c>
+      <c r="B405" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C405" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D405" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n" s="0">
+        <v>711.0</v>
+      </c>
+      <c r="B406" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C406" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D406" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n" s="0">
+        <v>712.0</v>
+      </c>
+      <c r="B407" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C407" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D407" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n" s="0">
+        <v>713.0</v>
+      </c>
+      <c r="B408" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C408" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D408" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n" s="0">
+        <v>714.0</v>
+      </c>
+      <c r="B409" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C409" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D409" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n" s="0">
+        <v>715.0</v>
+      </c>
+      <c r="B410" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C410" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D410" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n" s="0">
+        <v>716.0</v>
+      </c>
+      <c r="B411" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C411" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D411" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n" s="0">
+        <v>717.0</v>
+      </c>
+      <c r="B412" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C412" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D412" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n" s="0">
+        <v>718.0</v>
+      </c>
+      <c r="B413" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C413" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D413" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n" s="0">
+        <v>719.0</v>
+      </c>
+      <c r="B414" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C414" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D414" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n" s="0">
+        <v>720.0</v>
+      </c>
+      <c r="B415" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C415" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D415" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n" s="0">
+        <v>721.0</v>
+      </c>
+      <c r="B416" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C416" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D416" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n" s="0">
+        <v>722.0</v>
+      </c>
+      <c r="B417" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C417" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D417" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n" s="0">
+        <v>723.0</v>
+      </c>
+      <c r="B418" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C418" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D418" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n" s="0">
+        <v>724.0</v>
+      </c>
+      <c r="B419" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C419" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D419" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n" s="0">
+        <v>725.0</v>
+      </c>
+      <c r="B420" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C420" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D420" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n" s="0">
+        <v>726.0</v>
+      </c>
+      <c r="B421" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C421" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D421" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n" s="0">
+        <v>727.0</v>
+      </c>
+      <c r="B422" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C422" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D422" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n" s="0">
+        <v>728.0</v>
+      </c>
+      <c r="B423" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C423" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D423" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n" s="0">
+        <v>729.0</v>
+      </c>
+      <c r="B424" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C424" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D424" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n" s="0">
+        <v>730.0</v>
+      </c>
+      <c r="B425" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C425" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D425" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n" s="0">
+        <v>731.0</v>
+      </c>
+      <c r="B426" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C426" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D426" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n" s="0">
+        <v>732.0</v>
+      </c>
+      <c r="B427" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C427" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D427" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n" s="0">
+        <v>733.0</v>
+      </c>
+      <c r="B428" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C428" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D428" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n" s="0">
+        <v>734.0</v>
+      </c>
+      <c r="B429" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C429" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D429" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n" s="0">
+        <v>735.0</v>
+      </c>
+      <c r="B430" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C430" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D430" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n" s="0">
+        <v>736.0</v>
+      </c>
+      <c r="B431" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C431" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D431" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n" s="0">
+        <v>737.0</v>
+      </c>
+      <c r="B432" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C432" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D432" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n" s="0">
+        <v>738.0</v>
+      </c>
+      <c r="B433" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C433" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D433" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n" s="0">
+        <v>739.0</v>
+      </c>
+      <c r="B434" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C434" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D434" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n" s="0">
+        <v>740.0</v>
+      </c>
+      <c r="B435" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C435" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D435" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n" s="0">
+        <v>741.0</v>
+      </c>
+      <c r="B436" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C436" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D436" t="n" s="13">
+        <v>45625.0</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n" s="0">
+        <v>742.0</v>
+      </c>
+      <c r="B437" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C437" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D437" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n" s="0">
+        <v>743.0</v>
+      </c>
+      <c r="B438" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C438" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D438" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n" s="0">
+        <v>744.0</v>
+      </c>
+      <c r="B439" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C439" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D439" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n" s="0">
+        <v>745.0</v>
+      </c>
+      <c r="B440" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C440" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D440" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n" s="0">
+        <v>746.0</v>
+      </c>
+      <c r="B441" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C441" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D441" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n" s="0">
+        <v>747.0</v>
+      </c>
+      <c r="B442" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C442" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D442" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n" s="0">
+        <v>748.0</v>
+      </c>
+      <c r="B443" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C443" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D443" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n" s="0">
+        <v>749.0</v>
+      </c>
+      <c r="B444" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C444" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D444" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n" s="0">
+        <v>750.0</v>
+      </c>
+      <c r="B445" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C445" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D445" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n" s="0">
+        <v>751.0</v>
+      </c>
+      <c r="B446" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C446" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D446" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n" s="0">
+        <v>752.0</v>
+      </c>
+      <c r="B447" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C447" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D447" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n" s="0">
+        <v>753.0</v>
+      </c>
+      <c r="B448" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C448" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D448" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n" s="0">
+        <v>754.0</v>
+      </c>
+      <c r="B449" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C449" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D449" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n" s="0">
+        <v>755.0</v>
+      </c>
+      <c r="B450" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C450" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D450" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n" s="0">
+        <v>756.0</v>
+      </c>
+      <c r="B451" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C451" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D451" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n" s="0">
+        <v>757.0</v>
+      </c>
+      <c r="B452" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C452" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D452" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n" s="0">
+        <v>758.0</v>
+      </c>
+      <c r="B453" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C453" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D453" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n" s="0">
+        <v>759.0</v>
+      </c>
+      <c r="B454" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C454" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D454" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n" s="0">
+        <v>760.0</v>
+      </c>
+      <c r="B455" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C455" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D455" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n" s="0">
+        <v>761.0</v>
+      </c>
+      <c r="B456" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C456" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D456" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n" s="0">
+        <v>762.0</v>
+      </c>
+      <c r="B457" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C457" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D457" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n" s="0">
+        <v>763.0</v>
+      </c>
+      <c r="B458" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C458" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D458" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n" s="0">
+        <v>764.0</v>
+      </c>
+      <c r="B459" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C459" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D459" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n" s="0">
+        <v>765.0</v>
+      </c>
+      <c r="B460" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C460" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D460" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n" s="0">
+        <v>766.0</v>
+      </c>
+      <c r="B461" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C461" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D461" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="B462" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C462" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D462" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n" s="0">
+        <v>768.0</v>
+      </c>
+      <c r="B463" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C463" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D463" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n" s="0">
+        <v>769.0</v>
+      </c>
+      <c r="B464" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C464" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D464" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n" s="0">
+        <v>770.0</v>
+      </c>
+      <c r="B465" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C465" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D465" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n" s="0">
+        <v>771.0</v>
+      </c>
+      <c r="B466" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C466" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D466" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n" s="0">
+        <v>772.0</v>
+      </c>
+      <c r="B467" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C467" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D467" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n" s="0">
+        <v>773.0</v>
+      </c>
+      <c r="B468" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C468" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D468" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n" s="0">
+        <v>774.0</v>
+      </c>
+      <c r="B469" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C469" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D469" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n" s="0">
+        <v>775.0</v>
+      </c>
+      <c r="B470" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C470" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D470" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n" s="0">
+        <v>776.0</v>
+      </c>
+      <c r="B471" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C471" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D471" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n" s="0">
+        <v>777.0</v>
+      </c>
+      <c r="B472" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C472" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D472" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n" s="0">
+        <v>778.0</v>
+      </c>
+      <c r="B473" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C473" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D473" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n" s="0">
+        <v>779.0</v>
+      </c>
+      <c r="B474" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C474" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D474" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n" s="0">
+        <v>780.0</v>
+      </c>
+      <c r="B475" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C475" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D475" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n" s="0">
+        <v>781.0</v>
+      </c>
+      <c r="B476" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C476" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D476" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n" s="0">
+        <v>782.0</v>
+      </c>
+      <c r="B477" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C477" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D477" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n" s="0">
+        <v>783.0</v>
+      </c>
+      <c r="B478" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C478" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D478" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n" s="0">
+        <v>784.0</v>
+      </c>
+      <c r="B479" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C479" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D479" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n" s="0">
+        <v>785.0</v>
+      </c>
+      <c r="B480" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C480" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D480" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n" s="0">
+        <v>786.0</v>
+      </c>
+      <c r="B481" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C481" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D481" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n" s="0">
+        <v>787.0</v>
+      </c>
+      <c r="B482" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C482" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D482" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n" s="0">
+        <v>788.0</v>
+      </c>
+      <c r="B483" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C483" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D483" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n" s="0">
+        <v>789.0</v>
+      </c>
+      <c r="B484" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C484" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D484" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n" s="0">
+        <v>790.0</v>
+      </c>
+      <c r="B485" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C485" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D485" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n" s="0">
+        <v>791.0</v>
+      </c>
+      <c r="B486" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C486" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D486" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n" s="0">
+        <v>792.0</v>
+      </c>
+      <c r="B487" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C487" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D487" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n" s="0">
+        <v>793.0</v>
+      </c>
+      <c r="B488" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C488" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D488" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n" s="0">
+        <v>794.0</v>
+      </c>
+      <c r="B489" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C489" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D489" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n" s="0">
+        <v>795.0</v>
+      </c>
+      <c r="B490" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C490" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D490" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n" s="0">
+        <v>796.0</v>
+      </c>
+      <c r="B491" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C491" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D491" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n" s="0">
+        <v>797.0</v>
+      </c>
+      <c r="B492" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C492" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D492" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n" s="0">
+        <v>798.0</v>
+      </c>
+      <c r="B493" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C493" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D493" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n" s="0">
+        <v>799.0</v>
+      </c>
+      <c r="B494" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C494" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D494" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n" s="0">
+        <v>800.0</v>
+      </c>
+      <c r="B495" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C495" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D495" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n" s="0">
+        <v>801.0</v>
+      </c>
+      <c r="B496" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C496" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D496" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n" s="0">
+        <v>802.0</v>
+      </c>
+      <c r="B497" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C497" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D497" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n" s="0">
+        <v>803.0</v>
+      </c>
+      <c r="B498" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C498" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D498" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n" s="0">
+        <v>804.0</v>
+      </c>
+      <c r="B499" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C499" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D499" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n" s="0">
+        <v>805.0</v>
+      </c>
+      <c r="B500" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C500" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D500" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n" s="0">
+        <v>806.0</v>
+      </c>
+      <c r="B501" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C501" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D501" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n" s="0">
+        <v>807.0</v>
+      </c>
+      <c r="B502" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C502" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D502" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="n" s="0">
+        <v>808.0</v>
+      </c>
+      <c r="B503" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C503" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D503" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="n" s="0">
+        <v>809.0</v>
+      </c>
+      <c r="B504" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C504" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D504" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="n" s="0">
+        <v>810.0</v>
+      </c>
+      <c r="B505" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C505" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D505" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="n" s="0">
+        <v>811.0</v>
+      </c>
+      <c r="B506" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C506" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D506" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="n" s="0">
+        <v>812.0</v>
+      </c>
+      <c r="B507" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C507" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D507" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="n" s="0">
+        <v>813.0</v>
+      </c>
+      <c r="B508" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C508" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D508" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="n" s="0">
+        <v>814.0</v>
+      </c>
+      <c r="B509" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C509" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D509" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="n" s="0">
+        <v>815.0</v>
+      </c>
+      <c r="B510" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C510" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D510" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="n" s="0">
+        <v>816.0</v>
+      </c>
+      <c r="B511" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C511" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D511" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="n" s="0">
+        <v>817.0</v>
+      </c>
+      <c r="B512" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C512" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D512" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="n" s="0">
+        <v>818.0</v>
+      </c>
+      <c r="B513" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C513" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D513" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="n" s="0">
+        <v>819.0</v>
+      </c>
+      <c r="B514" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C514" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D514" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="n" s="0">
+        <v>820.0</v>
+      </c>
+      <c r="B515" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C515" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D515" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="n" s="0">
+        <v>821.0</v>
+      </c>
+      <c r="B516" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C516" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D516" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="n" s="0">
+        <v>822.0</v>
+      </c>
+      <c r="B517" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C517" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D517" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="n" s="0">
+        <v>823.0</v>
+      </c>
+      <c r="B518" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C518" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D518" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="n" s="0">
+        <v>824.0</v>
+      </c>
+      <c r="B519" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C519" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D519" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="n" s="0">
+        <v>825.0</v>
+      </c>
+      <c r="B520" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C520" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D520" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="n" s="0">
+        <v>826.0</v>
+      </c>
+      <c r="B521" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C521" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D521" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="n" s="0">
+        <v>827.0</v>
+      </c>
+      <c r="B522" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C522" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D522" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="n" s="0">
+        <v>828.0</v>
+      </c>
+      <c r="B523" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C523" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D523" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="n" s="0">
+        <v>829.0</v>
+      </c>
+      <c r="B524" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C524" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D524" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="n" s="0">
+        <v>830.0</v>
+      </c>
+      <c r="B525" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C525" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D525" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="n" s="0">
+        <v>831.0</v>
+      </c>
+      <c r="B526" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C526" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D526" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="n" s="0">
+        <v>832.0</v>
+      </c>
+      <c r="B527" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C527" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D527" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="n" s="0">
+        <v>833.0</v>
+      </c>
+      <c r="B528" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C528" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D528" t="n" s="13">
+        <v>45627.0</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="n" s="0">
+        <v>834.0</v>
+      </c>
+      <c r="B529" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C529" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D529" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="n" s="0">
+        <v>835.0</v>
+      </c>
+      <c r="B530" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C530" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D530" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="n" s="0">
+        <v>836.0</v>
+      </c>
+      <c r="B531" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C531" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D531" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="n" s="0">
+        <v>837.0</v>
+      </c>
+      <c r="B532" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C532" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D532" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="n" s="0">
+        <v>838.0</v>
+      </c>
+      <c r="B533" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C533" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D533" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="n" s="0">
+        <v>839.0</v>
+      </c>
+      <c r="B534" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C534" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D534" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="n" s="0">
+        <v>840.0</v>
+      </c>
+      <c r="B535" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C535" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D535" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="n" s="0">
+        <v>841.0</v>
+      </c>
+      <c r="B536" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C536" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D536" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="n" s="0">
+        <v>842.0</v>
+      </c>
+      <c r="B537" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C537" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D537" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="n" s="0">
+        <v>843.0</v>
+      </c>
+      <c r="B538" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C538" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D538" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="n" s="0">
+        <v>844.0</v>
+      </c>
+      <c r="B539" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C539" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D539" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="n" s="0">
+        <v>845.0</v>
+      </c>
+      <c r="B540" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C540" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D540" t="n" s="13">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="n" s="0">
+        <v>846.0</v>
+      </c>
+      <c r="B541" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C541" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D541" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="n" s="0">
+        <v>847.0</v>
+      </c>
+      <c r="B542" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C542" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D542" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="n" s="0">
+        <v>848.0</v>
+      </c>
+      <c r="B543" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C543" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D543" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="n" s="0">
+        <v>849.0</v>
+      </c>
+      <c r="B544" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C544" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D544" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="n" s="0">
+        <v>850.0</v>
+      </c>
+      <c r="B545" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C545" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D545" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="n" s="0">
+        <v>851.0</v>
+      </c>
+      <c r="B546" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C546" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D546" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="n" s="0">
+        <v>852.0</v>
+      </c>
+      <c r="B547" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C547" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D547" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="n" s="0">
+        <v>853.0</v>
+      </c>
+      <c r="B548" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C548" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D548" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="n" s="0">
+        <v>854.0</v>
+      </c>
+      <c r="B549" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C549" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D549" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="n" s="0">
+        <v>855.0</v>
+      </c>
+      <c r="B550" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C550" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D550" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="n" s="0">
+        <v>856.0</v>
+      </c>
+      <c r="B551" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C551" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D551" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="n" s="0">
+        <v>857.0</v>
+      </c>
+      <c r="B552" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C552" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D552" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="n" s="0">
+        <v>858.0</v>
+      </c>
+      <c r="B553" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C553" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D553" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="n" s="0">
+        <v>859.0</v>
+      </c>
+      <c r="B554" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C554" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D554" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="n" s="0">
+        <v>860.0</v>
+      </c>
+      <c r="B555" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C555" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D555" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="n" s="0">
+        <v>861.0</v>
+      </c>
+      <c r="B556" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C556" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D556" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="n" s="0">
+        <v>862.0</v>
+      </c>
+      <c r="B557" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C557" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D557" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="n" s="0">
+        <v>863.0</v>
+      </c>
+      <c r="B558" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C558" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D558" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="n" s="0">
+        <v>864.0</v>
+      </c>
+      <c r="B559" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C559" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D559" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="n" s="0">
+        <v>865.0</v>
+      </c>
+      <c r="B560" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C560" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D560" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="n" s="0">
+        <v>866.0</v>
+      </c>
+      <c r="B561" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C561" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D561" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="n" s="0">
+        <v>867.0</v>
+      </c>
+      <c r="B562" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C562" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D562" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="n" s="0">
+        <v>868.0</v>
+      </c>
+      <c r="B563" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C563" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D563" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="n" s="0">
+        <v>869.0</v>
+      </c>
+      <c r="B564" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C564" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D564" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="n" s="0">
+        <v>870.0</v>
+      </c>
+      <c r="B565" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C565" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D565" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="n" s="0">
+        <v>871.0</v>
+      </c>
+      <c r="B566" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C566" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D566" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="n" s="0">
+        <v>872.0</v>
+      </c>
+      <c r="B567" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C567" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D567" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="n" s="0">
+        <v>873.0</v>
+      </c>
+      <c r="B568" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C568" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D568" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="n" s="0">
+        <v>874.0</v>
+      </c>
+      <c r="B569" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C569" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D569" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="n" s="0">
+        <v>875.0</v>
+      </c>
+      <c r="B570" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C570" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D570" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="n" s="0">
+        <v>876.0</v>
+      </c>
+      <c r="B571" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C571" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D571" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="n" s="0">
+        <v>877.0</v>
+      </c>
+      <c r="B572" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C572" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D572" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="n" s="0">
+        <v>878.0</v>
+      </c>
+      <c r="B573" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C573" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D573" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="n" s="0">
+        <v>879.0</v>
+      </c>
+      <c r="B574" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C574" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D574" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="n" s="0">
+        <v>880.0</v>
+      </c>
+      <c r="B575" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C575" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D575" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="n" s="0">
+        <v>881.0</v>
+      </c>
+      <c r="B576" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C576" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D576" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="n" s="0">
+        <v>882.0</v>
+      </c>
+      <c r="B577" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C577" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D577" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="n" s="0">
+        <v>883.0</v>
+      </c>
+      <c r="B578" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C578" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D578" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="n" s="0">
+        <v>884.0</v>
+      </c>
+      <c r="B579" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C579" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D579" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="n" s="0">
+        <v>885.0</v>
+      </c>
+      <c r="B580" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C580" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D580" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="n" s="0">
+        <v>886.0</v>
+      </c>
+      <c r="B581" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C581" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D581" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="n" s="0">
+        <v>887.0</v>
+      </c>
+      <c r="B582" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C582" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D582" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="n" s="0">
+        <v>888.0</v>
+      </c>
+      <c r="B583" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C583" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D583" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="n" s="0">
+        <v>889.0</v>
+      </c>
+      <c r="B584" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C584" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D584" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="n" s="0">
+        <v>890.0</v>
+      </c>
+      <c r="B585" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C585" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D585" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="n" s="0">
+        <v>891.0</v>
+      </c>
+      <c r="B586" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C586" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D586" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="n" s="0">
+        <v>892.0</v>
+      </c>
+      <c r="B587" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C587" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D587" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="n" s="0">
+        <v>893.0</v>
+      </c>
+      <c r="B588" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C588" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D588" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="n" s="0">
+        <v>894.0</v>
+      </c>
+      <c r="B589" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C589" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D589" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="n" s="0">
+        <v>895.0</v>
+      </c>
+      <c r="B590" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C590" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D590" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="n" s="0">
+        <v>896.0</v>
+      </c>
+      <c r="B591" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C591" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D591" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="n" s="0">
+        <v>897.0</v>
+      </c>
+      <c r="B592" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C592" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D592" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="n" s="0">
+        <v>898.0</v>
+      </c>
+      <c r="B593" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C593" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D593" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="n" s="0">
+        <v>899.0</v>
+      </c>
+      <c r="B594" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C594" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D594" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="n" s="0">
+        <v>900.0</v>
+      </c>
+      <c r="B595" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C595" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D595" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="n" s="0">
+        <v>901.0</v>
+      </c>
+      <c r="B596" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C596" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D596" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="n" s="0">
+        <v>902.0</v>
+      </c>
+      <c r="B597" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C597" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D597" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="n" s="0">
+        <v>903.0</v>
+      </c>
+      <c r="B598" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C598" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D598" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="n" s="0">
+        <v>904.0</v>
+      </c>
+      <c r="B599" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C599" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D599" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="n" s="0">
+        <v>905.0</v>
+      </c>
+      <c r="B600" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C600" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D600" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="n" s="0">
+        <v>906.0</v>
+      </c>
+      <c r="B601" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C601" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D601" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="n" s="0">
+        <v>907.0</v>
+      </c>
+      <c r="B602" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C602" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D602" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="n" s="0">
+        <v>908.0</v>
+      </c>
+      <c r="B603" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C603" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D603" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="n" s="0">
+        <v>909.0</v>
+      </c>
+      <c r="B604" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C604" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D604" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="n" s="0">
+        <v>910.0</v>
+      </c>
+      <c r="B605" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C605" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D605" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="n" s="0">
+        <v>911.0</v>
+      </c>
+      <c r="B606" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C606" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D606" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="n" s="0">
+        <v>912.0</v>
+      </c>
+      <c r="B607" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C607" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D607" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="n" s="0">
+        <v>913.0</v>
+      </c>
+      <c r="B608" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C608" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D608" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="n" s="0">
+        <v>914.0</v>
+      </c>
+      <c r="B609" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C609" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D609" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="n" s="0">
+        <v>915.0</v>
+      </c>
+      <c r="B610" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C610" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D610" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="n" s="0">
+        <v>916.0</v>
+      </c>
+      <c r="B611" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C611" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D611" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="n" s="0">
+        <v>917.0</v>
+      </c>
+      <c r="B612" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C612" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D612" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="n" s="0">
+        <v>918.0</v>
+      </c>
+      <c r="B613" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C613" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D613" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="n" s="0">
+        <v>919.0</v>
+      </c>
+      <c r="B614" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C614" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D614" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="n" s="0">
+        <v>920.0</v>
+      </c>
+      <c r="B615" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C615" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D615" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="n" s="0">
+        <v>921.0</v>
+      </c>
+      <c r="B616" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C616" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D616" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="n" s="0">
+        <v>922.0</v>
+      </c>
+      <c r="B617" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C617" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D617" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="n" s="0">
+        <v>923.0</v>
+      </c>
+      <c r="B618" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C618" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D618" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="n" s="0">
+        <v>924.0</v>
+      </c>
+      <c r="B619" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C619" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D619" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="n" s="0">
+        <v>925.0</v>
+      </c>
+      <c r="B620" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C620" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D620" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="n" s="0">
+        <v>926.0</v>
+      </c>
+      <c r="B621" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C621" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D621" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="n" s="0">
+        <v>927.0</v>
+      </c>
+      <c r="B622" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C622" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D622" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="n" s="0">
+        <v>928.0</v>
+      </c>
+      <c r="B623" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C623" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D623" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="n" s="0">
+        <v>929.0</v>
+      </c>
+      <c r="B624" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C624" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D624" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="n" s="0">
+        <v>930.0</v>
+      </c>
+      <c r="B625" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C625" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D625" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="n" s="0">
+        <v>931.0</v>
+      </c>
+      <c r="B626" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C626" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D626" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="n" s="0">
+        <v>932.0</v>
+      </c>
+      <c r="B627" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C627" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D627" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="n" s="0">
+        <v>933.0</v>
+      </c>
+      <c r="B628" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C628" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D628" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="n" s="0">
+        <v>934.0</v>
+      </c>
+      <c r="B629" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C629" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D629" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="n" s="0">
+        <v>935.0</v>
+      </c>
+      <c r="B630" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C630" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D630" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="n" s="0">
+        <v>936.0</v>
+      </c>
+      <c r="B631" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C631" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D631" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="n" s="0">
+        <v>937.0</v>
+      </c>
+      <c r="B632" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C632" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D632" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="n" s="0">
+        <v>938.0</v>
+      </c>
+      <c r="B633" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C633" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D633" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="n" s="0">
+        <v>939.0</v>
+      </c>
+      <c r="B634" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C634" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D634" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="n" s="0">
+        <v>940.0</v>
+      </c>
+      <c r="B635" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C635" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D635" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="n" s="0">
+        <v>941.0</v>
+      </c>
+      <c r="B636" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C636" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D636" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="n" s="0">
+        <v>942.0</v>
+      </c>
+      <c r="B637" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C637" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D637" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="n" s="0">
+        <v>943.0</v>
+      </c>
+      <c r="B638" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C638" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D638" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="n" s="0">
+        <v>944.0</v>
+      </c>
+      <c r="B639" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C639" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D639" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="n" s="0">
+        <v>945.0</v>
+      </c>
+      <c r="B640" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C640" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D640" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="n" s="0">
+        <v>946.0</v>
+      </c>
+      <c r="B641" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C641" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D641" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="n" s="0">
+        <v>947.0</v>
+      </c>
+      <c r="B642" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C642" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D642" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="n" s="0">
+        <v>948.0</v>
+      </c>
+      <c r="B643" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C643" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D643" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="n" s="0">
+        <v>949.0</v>
+      </c>
+      <c r="B644" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C644" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D644" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="n" s="0">
+        <v>950.0</v>
+      </c>
+      <c r="B645" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C645" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D645" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="n" s="0">
+        <v>951.0</v>
+      </c>
+      <c r="B646" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C646" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D646" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="n" s="0">
+        <v>952.0</v>
+      </c>
+      <c r="B647" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C647" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D647" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="n" s="0">
+        <v>953.0</v>
+      </c>
+      <c r="B648" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C648" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D648" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="n" s="0">
+        <v>954.0</v>
+      </c>
+      <c r="B649" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C649" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D649" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="n" s="0">
+        <v>955.0</v>
+      </c>
+      <c r="B650" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C650" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D650" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="n" s="0">
+        <v>956.0</v>
+      </c>
+      <c r="B651" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C651" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D651" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="n" s="0">
+        <v>957.0</v>
+      </c>
+      <c r="B652" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C652" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D652" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="n" s="0">
+        <v>958.0</v>
+      </c>
+      <c r="B653" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C653" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D653" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="n" s="0">
+        <v>959.0</v>
+      </c>
+      <c r="B654" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C654" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D654" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="n" s="0">
+        <v>960.0</v>
+      </c>
+      <c r="B655" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C655" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D655" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="n" s="0">
+        <v>961.0</v>
+      </c>
+      <c r="B656" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C656" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D656" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="n" s="0">
+        <v>962.0</v>
+      </c>
+      <c r="B657" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C657" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D657" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="n" s="0">
+        <v>963.0</v>
+      </c>
+      <c r="B658" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C658" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D658" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="n" s="0">
+        <v>964.0</v>
+      </c>
+      <c r="B659" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C659" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D659" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="n" s="0">
+        <v>965.0</v>
+      </c>
+      <c r="B660" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C660" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D660" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="n" s="0">
+        <v>966.0</v>
+      </c>
+      <c r="B661" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C661" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D661" t="n" s="14">
+        <v>45628.0</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="n" s="0">
+        <v>967.0</v>
+      </c>
+      <c r="B662" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C662" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D662" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="n" s="0">
+        <v>968.0</v>
+      </c>
+      <c r="B663" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C663" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D663" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="n" s="0">
+        <v>969.0</v>
+      </c>
+      <c r="B664" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C664" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D664" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="n" s="0">
+        <v>970.0</v>
+      </c>
+      <c r="B665" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C665" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D665" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="n" s="0">
+        <v>971.0</v>
+      </c>
+      <c r="B666" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C666" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D666" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="n" s="0">
+        <v>972.0</v>
+      </c>
+      <c r="B667" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C667" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D667" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="n" s="0">
+        <v>973.0</v>
+      </c>
+      <c r="B668" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C668" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D668" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="n" s="0">
+        <v>974.0</v>
+      </c>
+      <c r="B669" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C669" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D669" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="n" s="0">
+        <v>975.0</v>
+      </c>
+      <c r="B670" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C670" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D670" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="n" s="0">
+        <v>976.0</v>
+      </c>
+      <c r="B671" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C671" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D671" t="n" s="14">
+        <v>45629.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rabbitmq ayarlamaları yapıldıancak message unacked de kalıyor düzeltilmesi lazım
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -263,12 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -615,7 +616,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D671"/>
+  <dimension ref="A1:D686"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -10023,6 +10024,216 @@
         <v>45629.0</v>
       </c>
     </row>
+    <row r="672">
+      <c r="A672" t="n" s="0">
+        <v>977.0</v>
+      </c>
+      <c r="B672" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C672" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D672" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="n" s="0">
+        <v>978.0</v>
+      </c>
+      <c r="B673" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C673" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D673" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="n" s="0">
+        <v>979.0</v>
+      </c>
+      <c r="B674" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C674" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D674" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="n" s="0">
+        <v>980.0</v>
+      </c>
+      <c r="B675" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C675" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D675" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="n" s="0">
+        <v>981.0</v>
+      </c>
+      <c r="B676" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C676" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D676" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="n" s="0">
+        <v>982.0</v>
+      </c>
+      <c r="B677" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C677" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D677" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="n" s="0">
+        <v>983.0</v>
+      </c>
+      <c r="B678" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C678" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D678" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="n" s="0">
+        <v>984.0</v>
+      </c>
+      <c r="B679" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C679" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D679" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="n" s="0">
+        <v>985.0</v>
+      </c>
+      <c r="B680" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C680" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D680" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="n" s="0">
+        <v>986.0</v>
+      </c>
+      <c r="B681" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C681" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D681" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="n" s="0">
+        <v>987.0</v>
+      </c>
+      <c r="B682" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C682" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D682" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="n" s="0">
+        <v>988.0</v>
+      </c>
+      <c r="B683" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C683" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D683" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="n" s="0">
+        <v>989.0</v>
+      </c>
+      <c r="B684" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C684" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D684" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="n" s="0">
+        <v>990.0</v>
+      </c>
+      <c r="B685" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C685" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D685" t="n" s="15">
+        <v>45630.0</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="n" s="0">
+        <v>991.0</v>
+      </c>
+      <c r="B686" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C686" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D686" t="n" s="15">
+        <v>45631.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>